<commit_message>
updates error boundary for more than 5 projects of a single candidate
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -469,15 +469,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The candidate lacks the required skills in MongoDB and NodeJS, which are crucial for the job. The projects demonstrate good proficiency in ReactJS and JavaScript, but the absence of MongoDB and NodeJS skills impacts the score.</t>
+          <t>The candidate lacks the required skills of MongoDB and NodeJS which are essential for the role. Their past projects show strong skills in Data Analysis and Computer Vision, but these do not directly align with the job requirements.</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The candidate has demonstrated strong adaptability, problem-solving skills, and a willingness to learn in the interview answers. Additionally, the candidate's interest in AI and the desire to contribute to cutting-edge technologies align well with the company's goals, but the preference to not work alone may need to be addressed.</t>
+          <t>The candidate shows good adaptability by expressing willingness to work in different countries, but may need to work on improving skills independently. The candidate's interest in learning new skills and contributing to cutting-edge technologies aligns with the company's expectations.</t>
         </is>
       </c>
     </row>
@@ -490,15 +490,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The candidate lacks the required skills of MongoDB and Web Development, which are essential for the role. Although they have experience with some relevant technologies, the absence of these key skills has impacted the score.</t>
+          <t>The candidate lacks the required skills in MongoDB, which is essential for the job. Additionally, the candidate has knowledge of Dart and Firebase, which are not mentioned in the job description.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The candidate demonstrates strong adaptability, teamwork, and problem-solving skills. Their eagerness to immerse in a new culture and work environment, along with a clear career plan, shows a positive attitude. The expressed interest in learning from the Japanese work culture and language also demonstrates flexibility and adaptability, making them a suitable candidate for the role.</t>
+          <t>The applicant has a strong motivation to work in Japan, demonstrated by the interest in AI, the desire to be part of Japanese work culture, and the willingness to learn a new language. The applicant also shows adaptability and a collaborative approach, which align with the company's values. However, the preference not to work alone and the need to improve skills may impact the overall personality score.</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The candidate lacks direct experience with MERN stack (MongoDB, ExpressJS, ReactJS, NodeJS) which are primary requirements for the job. However, the candidate's projects showcase strong skills in AI/ML, Python, and ReactJS, which could be beneficial in a tech-driven environment.</t>
+          <t>The applicant lacks the required skills of MongoDB and NodeJS, which are crucial for the MERN stack development role. The candidate excels in Python, PyTorch, Tensorflow, and Django Rest Framework, which are not directly relevant to the job description.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The candidate shows a strong interest in Japanese work culture and willingness to adapt to a new environment. The candidate also demonstrates good teamwork and problem-solving skills. However, there is room for improvement in time management and adaptability, which are important for working in a foreign country.</t>
+          <t>The applicant demonstrates enthusiasm for AI/ML and shows willingness to adapt to new cultures. They have good teamwork skills and a problem-solving attitude. However, they may need to work on independence and time management.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates prompt and results
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -469,15 +469,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The candidate lacks the required skills of MongoDB and NodeJS which are essential for the role. Their past projects show strong skills in Data Analysis and Computer Vision, but these do not directly align with the job requirements.</t>
+          <t>The applicant's projects extensively cover web development using ReactJS and includes experience in Django, Python, and JavaScript, which align with the required skills. However, the lack of experience with MongoDB and NodeJS, as required by the job, may have led to a slightly lower score.</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The candidate shows good adaptability by expressing willingness to work in different countries, but may need to work on improving skills independently. The candidate's interest in learning new skills and contributing to cutting-edge technologies aligns with the company's expectations.</t>
+          <t>The applicant shows strong adaptability, communication, teamwork, and problem-solving skills, as evidenced by the answers provided. Additionally, the willingness to work in Japan and openness to new cultures demonstrate a high level of adaptability and cultural awareness.</t>
         </is>
       </c>
     </row>
@@ -490,15 +490,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The candidate lacks the required skills in MongoDB, which is essential for the job. Additionally, the candidate has knowledge of Dart and Firebase, which are not mentioned in the job description.</t>
+          <t>The applicant has a good score because they have experience with NodeJS, ExpressJS, ReactJS, and Web Development, which align with the company's requirements. However, the lack of experience with MongoDB and JavaScript could be a drawback based on the job description.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The applicant has a strong motivation to work in Japan, demonstrated by the interest in AI, the desire to be part of Japanese work culture, and the willingness to learn a new language. The applicant also shows adaptability and a collaborative approach, which align with the company's values. However, the preference not to work alone and the need to improve skills may impact the overall personality score.</t>
+          <t>The applicant seems adaptable, willing to learn new skills, and is enthusiastic about being part of a new work culture. They also value teamwork and are open to working in Japan, making them a good fit for the company.</t>
         </is>
       </c>
     </row>
@@ -511,15 +511,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The applicant lacks the required skills of MongoDB and NodeJS, which are crucial for the MERN stack development role. The candidate excels in Python, PyTorch, Tensorflow, and Django Rest Framework, which are not directly relevant to the job description.</t>
+          <t>The applicant has experience in Python, PyTorch, Tensorflow, and ReactJS, which are relevant to the job's requirements. However, the lack of experience in MongoDB, ExpressJS, and NodeJS could have affected the score.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The applicant demonstrates enthusiasm for AI/ML and shows willingness to adapt to new cultures. They have good teamwork skills and a problem-solving attitude. However, they may need to work on independence and time management.</t>
+          <t>The applicant has displayed strong adaptability and willingness to work in Japan. The responses indicate good communication, teamwork, and problem-solving skills, aligning with the company's soft skill requirements.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updates prompts and results
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The applicant has a high score due to the relevant projects that showcase skills in ReactJS, JavaScript, and Python, which are in line with the required skills for the SDE Intern position. Additionally, the applicant has demonstrated proficiency in Computer Vision and Image Processing, which could add value to the company's projects. However, the applicant lacks experience with MongoDB and NodeJS, which are also essential for the role, resulting in a lower but still moderate score.</t>
+          <t>The applicant has a diverse set of technical skills including JavaScript, PyTorch, Django, Data Analysis, Computer Vision, Python, and TensorFlow. Although the applicant's projects do not directly mention experience with MongoDB or NodeJS, the projects showcase strong technical abilities in web development, backend development, AI/ML, and data analysis. The applicant's experience in developing user-friendly platforms and working on cutting-edge AI/ML technologies demonstrates the potential to excel in a Remote MERN stack developer intern role.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The applicant demonstrates strong communication skills, adaptability, and a willingness to learn new skills, as evidenced by the desire to work in Japan to experience a new work culture and learn a new language. The applicant's collaborative nature, problem-solving approach, and ability to bridge the gap between technical and creative aspects in projects showcase strong teamwork and problem-solving skills. Hence, a score of 4 is suitable based on the applicant's personality and willingness to work in Japan.</t>
+          <t>The applicant has expressed a strong interest in working in Japan and has demonstrated adaptability and willingness to embrace a new culture. The applicant's eagerness to learn a new language, appreciation of Japanese work culture, and openness to working in diverse locations showcase a positive attitude. Furthermore, the applicant's collaborative problem-solving approach and the ability to bridge the gap between technical and creative aspects highlight strong teamwork and problem-solving skills. Based on the provided answers, the applicant exhibits strong potential for adapting to a new work environment in Japan, thus deserving a score of 4.</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The applicant has been given a score based on the projects and skills which align with the job description. The applicant has experience with web and mobile application development using technologies such as Flutter, Dart, Firebase, NodeJS, ExpressJS, ReactJS, WebRTC, HTML, and CSS. Although the applicant's projects do not directly align with the specific technologies mentioned in the job description such as MongoDB, the applicant's experience with web and mobile application development using NodeJS, ExpressJS, ReactJS, and other relevant technologies demonstrates a strong skill set that is transferable to the job requirements. It is evident that the applicant has a good understanding of web development and possesses a variety of relevant technical skills. The score reflects the alignment of the applicant's projects and skills with the responsibilities and requirements of the SDE Intern position.</t>
+          <t>The applicant has worked on diverse projects that showcase proficiency in web development and real-time application development, aligning with the job description's emphasis on web/mobile applications using MongoDB, ExpressJS, ReactJS, and NodeJS. The SHAMIYANA APP demonstrates skills in Flutter, Dart, and Firebase, while the RAPID project exhibits expertise in NodeJS, ExpressJS, Socket.IO, WebRTC, and Docker. Moreover, the SMART SENSING MIDDLEWARE project illustrates competence in ReactJS, HTML, and CSS, which are relevant to web development. Although the applicant lacks experience specifically with MongoDB, their strong foundation in web technologies and real-time applications positions them as a highly suitable candidate for the SDE Intern role.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The applicant has demonstrated a strong interest in working in Japan and adapting to a new culture. Their responses indicate a positive attitude towards embracing the work culture in Japan and learning a new language. They have expressed willingness to work in various countries, including Japan, and are confident about adapting to new cultures. Additionally, the applicant acknowledges their strengths in teamwork and communication, essential soft skills required for the job. Overall, the applicant's responses reflect a positive attitude, adaptability, and willingness to work in Japan, leading to a score of 4 out of 5.</t>
+          <t>The applicant has expressed a strong interest in Japan and its work culture, demonstrating adaptability and a willingness to embrace new experiences. Additionally, the applicant's emphasis on team collaboration and problem-solving, as evidenced by their response to overcoming technical challenges, signifies a favorable personality fit for the company. Therefore, the applicant is given a score of 4 for demonstrating a positive attitude towards working in Japan and exhibiting key soft skills sought by the company.</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The applicant has been given a score based on the relevance of his projects and skills to the job description. The applicant's projects demonstrate experience in computer vision, machine learning, and web development, which are valuable for the SDE Intern position. Although the applicant's skills cover a wide range of technologies, including Python, PyTorch, Tensorflow, and ReactJS, there is a lack of direct experience with MongoDB, ExpressJS, and NodeJS, which are crucial for this role. Therefore, the score has been calculated based on the strong technical background in relevant areas and the slight lack of experience with specific technologies required by the company.</t>
+          <t>The applicant has strong technical skills in Python, PyTorch, Tensorflow, and ReactJS which align well with the company's requirements. Although the applicant lacks direct experience in MongoDB, ExpressJS, and NodeJS, the applicant's expertise in web development and JavaScript, as well as experience with similar technologies, demonstrates the ability to quickly adapt and learn new technologies. The applicant's projects showcase a blend of machine learning, web development, and AI, indicating a diverse skill set that can contribute to high-quality web/mobile applications. The applicant's score reflects the alignment of their skills and project experiences with the job responsibilities and technical requirements.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Based on the applicant's answers and considering the soft skills that the company is looking for, I would rate the applicant 4 out of 5. The applicant has demonstrated good adaptability, communication skills, and expressed a willingness to work in Japan. Additionally, the applicant has shown a collaborative approach to problem-solving and emphasized the importance of teamwork. However, the applicant mentioned a preference not to work alone, which could be a potential area for improvement in terms of independence and self-reliance.</t>
+          <t>The applicant has displayed strong communication skills by articulating a clear desire to be part of Japan's work culture and expressing willingness to adapt to new cultures. Their commitment to learning new skills and the ability to work well in a team is evident from their responses. Furthermore, their demonstration of problem-solving abilities during challenging project situations signifies their potential to handle complexities in a new work environment. Overall, the applicant's responses convey a positive attitude and a strong willingness to work in Japan, earning them a score of 4.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates personality score reasons
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The applicant has strong skills in ReactJS and JavaScript, which are required for the job. Additionally, the applicant has experience in web development using Django and Python, which can be beneficial for the role. However, the job requires expertise in MongoDB and NodeJS, which are not explicitly mentioned in the applicant's projects or skills. Furthermore, the applicant lacks specific experience in MongoDB and NodeJS, which are essential for the position. Although the applicant's projects showcase proficiency in ReactJS and JavaScript, the absence of direct experience in MongoDB and NodeJS could impact the applicant's suitability for the role.</t>
+          <t>The applicant's projects demonstrate strong skills in ReactJS, Django, Python, and JavaScript, all of which are highly relevant to the job description. The applicant has experience in developing web applications and backend systems, displaying proficiency in MongoDB, ExpressJS, and NodeJS. Additionally, the applicant has worked on projects involving computer vision and image processing, showcasing a diverse skill set. However, the applicant lacks direct experience with MongoDB, which is a required skill for the job. While the applicant's projects demonstrate strong technical skills, the lack of direct MongoDB experience could be a potential area for further development.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Based on the applicant's responses and demonstrated adaptability, it is evident that the applicant possesses strong communication and problem-solving skills. The applicant's willingness to learn from the Japanese work culture and the ability to adapt to diverse cultures indicate a high level of adaptability and open-mindedness. Furthermore, the applicant's conscious effort to seek feedback and implement it, as well as the desire for continuous improvement, reflects a strong commitment to personal and professional growth. Overall, the applicant demonstrates a willingness to work in Japan and exhibits positive personality traits, warranting a score of 4 out of 5.</t>
+          <t>The applicant has demonstrated a willingness to learn, grow, and adapt through proactive participation in workshops and online courses to enhance skills. The applicant also exhibits a strong commitment to self-improvement and learning from setbacks, indicating good problem-solving skills and adaptability. The applicant's expressed interest in Japanese work culture and values, as well as their desire to work in Japan, align well with the company's cultural expectations. The applicant's detailed expectations from the company and clear career plan reflect strong communication and time management skills. Overall, the applicant's responses indicate a positive attitude, adaptability, and a strong alignment with the company's soft skill requirements.</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The applicant has a strong set of technical skills including ReactJS, NodeJS, ExpressJS, HTML, CSS, and WebRTC which are relevant to the job description. However, the applicant lacks experience with MongoDB and could benefit from gaining more exposure to this technology. Although the projects the applicant has worked on demonstrate proficiency in web and mobile application development, the absence of MongoDB in the projects may raise some concerns about the candidate's hands-on experience with the technology required by the company. Overall, the applicant's technical skills align well with the job requirements, but there is room for improvement in MongoDB.</t>
+          <t>The applicant has a high level of skill in ReactJS, NodeJS, and WebRTC, which are all relevant to the job requirements. Although the applicant does not have direct experience with MongoDB, the candidate's experience with Firebase, Docker, and ExpressJS demonstrates a strong foundation in database management and backend development, which can be transferrable to working with MongoDB. The applicant's project experience in developing a time-saving food delivery platform and a web app for real-time gaming and video calling shows the ability to work on web and mobile applications, which aligns with the responsibilities of the SDE Intern position. The use of technologies like Flutter, Dart, and ReactJS in the 'SHAMIYANA APP' project indicates the ability to work on front-end development. Overall, the applicant's diverse skill set and experience make them well-suited for the role, earning a high score.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The applicant has expressed a strong interest in working in Japan, highlighting the appeal of Japan's work culture and expressing a willingness to adapt to a new environment. The applicant has also demonstrated the ability to work collaboratively and has highlighted the value of teamwork and open communication. These qualities align with the soft skills the company is seeking, indicating a good fit in terms of adaptability and teamwork. Overall, the applicant's responses and attitudes suggest a positive willingness to work in Japan, earning a score of 4.</t>
+          <t>Based on the applicant's answers, it is evident that the applicant possesses strong communication skills as reflected in the clear articulation of career plans and expectations from the company. The applicant also expresses a willingness to adapt to new cultures and an interest in learning new skills, illustrating strong adaptability. Additionally, the applicant's acknowledgment of strengths in teamwork and open communication, along with the ability to address challenges collaboratively, demonstrates good problem-solving and teamwork skills. Overall, the applicant's responses reflect a positive attitude, strong teamwork skills, and adaptability, warranting a score of 4.</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The applicant possesses strong technical skills in Python, Django Rest Framework, ReactJS, PyTorch, and Tensorflow, which demonstrate proficiency in web and machine learning technologies. However, the job requires expertise in MongoDB, ExpressJS, and NodeJS, which are not evident from the applicant's projects. Additionally, the applicant lacks experience in web/mobile application development using the MERN stack as per the company's requirements.</t>
+          <t>The applicant has worked on several projects showcasing strong technical skills, including computer vision, image processing, and backend development using Django Rest Framework and ReactJS. While the specific skills required by the company, such as MongoDB and NodeJS, are not directly demonstrated in the projects, the applicant's broad skill set and experience with related technologies make them well-equipped to learn and adapt to the company's tech stack. The applicant's experience in predicting human activities using data analysis and machine learning aligns with the company's focus on web/mobile applications and product enhancement suggestions, demonstrating their potential to contribute effectively to the role.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The applicant's responses reflect a high level of adaptability, as well as a positive attitude towards learning and working within a new cultural setting like Japan. The applicant's strong teamwork skills and willingness to address weaknesses indicate a good fit for the company's requirements. Overall, the applicant's positive attitude and adaptability make them suitable for the role and working in Japan.</t>
+          <t>The applicant has exhibited strong communication skills, expressing eagerness to immerse themselves in Japan's AI industry and adapt to a new culture. Their interest in contributing to cutting-edge AI/ML technologies and desire to learn new skills align with the company's emphasis on problem solving and adaptability. The applicant's ability to recognize the importance of collaboration and open communication, as evidenced by their experience with project setbacks, indicates their potential to excel in a team-oriented environment. Given their positive attitude towards adapting to different cultures and their clear career goals, the applicant demonstrates a high level of enthusiasm and adaptability, earning a score of 4 out of 5 for their willingness to work in Japan.</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The applicant has strong skills in JavaScript, HTML, CSS, and API integration, which are essential for web development. While the applicant's projects do not specifically mention MERN stack technologies, the experience in developing web and mobile applications, messaging, file sharing, and screen sharing/recording demonstrate a strong foundation in web development. The applicant's background in engineering and graphic design sets them apart and showcases their ability to bridge technical and creative aspects in projects.</t>
+          <t>The applicant has good experience working on web development projects such as the Video Conferencing Project, TEDxIITGuwahati Website, and the Alcheringa Pass Portal, which involved JavaScript, HTML, and CSS. These projects demonstrate the applicant's ability to work with front-end technologies and API integration. Although the applicant's projects do not directly align with the MERN stack, the skills obtained from these projects are transferrable and can be utilized in the internship. The applicant has experience in API integration, JavaScript, HTML, and CSS, which are crucial for web development. Overall, the applicant's projects showcase a strong foundation in web development and the ability to work with relevant technologies, indicating a good potential fit for the MERN Stack Developer Internship. However, the applicant could benefit from further experience with MongoDB, ExpressJS, and NodeJS to fully align with the job requirements.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -540,7 +540,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The applicant has demonstrated strong communication skills, adaptability, and a willingness to work in Japan. They have expressed a keen interest in Japan's AI field and work culture. Additionally, the applicant has emphasized their ability to adapt to new cultures and learn a new language while working in Japan. Their commitment to collaborating within a team and addressing weaknesses also shows a positive attitude towards personal and professional growth.</t>
+          <t>Based on the applicant's responses, it is evident that they possess excellent communication skills and demonstrate a willingness to adapt to new cultures. The applicant's interest in being part of Japan's work culture and their openness to working in various countries showcase a strong level of adaptability. Additionally, the applicant has emphasized the importance of teamwork and collaboration, reflecting positive attributes that align with the company's soft skill requirements. The applicant's proactive approach to addressing weaknesses and their ability to learn from challenges further illustrate their problem-solving skills. Overall, the applicant exhibits strong attributes that align with the company's soft skill requirements and shows a high level of willingness to work in Japan.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adds wrapper for Data Manager
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -469,15 +469,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The applicant possesses strong skills in Python, JavaScript, ReactJS, and Django, which align well with the requirements for the SDE Intern position. The applicant's experience in developing web and mobile applications using ReactJS and Django, and utilizing PyTorch, Sklearn, and Python for data analysis demonstrates a solid technical foundation. However, the applicant lacks direct experience with MongoDB and NodeJS, which are key requirements for the role. While the applicant has demonstrated proficiency in similar technologies, additional training or experience in MongoDB and NodeJS may be beneficial for ensuring a seamless fit into the role. Overall, the applicant's technical expertise and project experience make them a strong candidate for the position, with the potential for further development in MongoDB and NodeJS.</t>
+          <t>The applicant possesses several key skills required by the company such as ReactJS, JavaScript, and some level of web development experience. While the applicant's projects are not directly in line with the company's requirements, the projects demonstrate a strong grasp of relevant technologies including ReactJS, Django, Python, JavaScript, and Computer Vision. However, the applicant lacks direct experience with MongoDB and NodeJS which are important for this role. Overall, the applicant has a good foundation in relevant technologies and has demonstrated the ability to learn new skills, presenting a strong case for potential success in the role.</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Based on the applicant's responses, it's evident that they exhibit strong adaptability, problem-solving skills, and a willingness to learn and improve. Their expressed interest in learning from the Japanese work culture, seeking feedback, and actively participating in relevant workshops and online courses demonstrates a proactive approach to personal and professional growth. The applicant's ability to overcome setbacks and their curiosity-driven mindset further reinforce their adaptability and problem-solving acumen. Additionally, their articulated vision for contributing to the company's goals, expectations from the company, and desire to immerse themselves in Japanese culture reflect a positive attitude and alignment with the company's values. The applicant's responses indicate a high level of motivation, adaptability, and a sincere interest in working in Japan.</t>
+          <t>The applicant demonstrates strong communication skills and a willingness to learn from Japanese work culture, indicating adaptability and a positive attitude towards working in Japan. Moreover, the applicant's emphasis on seeking feedback, continuous self-improvement, and desire to experience Japanese cultural values align well with the company's soft skills requirements. The applicant's clear expression of interest in working in Japan further strengthens the likelihood of successful integration into the work culture.</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The applicant has worked on projects that showcase his expertise in web and mobile application development. While the technologies used in the projects are not an exact match with the required skills of MongoDB, ExpressJS, ReactJS, and NodeJS, the applicant's skills in Flutter, Dart, WebRTC, Socket.IO, and HTML demonstrate an aptitude for web and mobile development. However, there is a gap in the required skills as the applicant lacks proficiency in MongoDB and JavaScript, which are essential for the role. Despite this, the applicant's diverse skill set and experience in developing functional applications display potential for growth and adaptability to the technologies used by the company.</t>
+          <t>The candidate has a strong technical background with experience in web and mobile application development utilizing technologies such as Flutter, Dart, Firebase, ReactJS, NodeJS, HTML, CSS, and WebRTC. Although the applicant's project experience primarily involves technologies such as Flutter, Dart, and Firebase, the candidate has demonstrated adaptability by working on a variety of projects involving different technology stacks. However, the required skills for the role include MongoDB, ExpressJS, and JavaScript, which are not directly reflected in the candidate's projects. While the candidate's projects showcase proficiency in relevant web and mobile technologies, there is a gap in direct experience with the specific technology stack mentioned in the job description. Despite this, the candidate's diverse skill set and demonstrated ability to learn new technologies provide a strong foundation for success in the role.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The applicant has expressed a deep interest in working in Japan, citing the country's leading position in AI and expressing fascination with the work culture. The applicant has also demonstrated openness to adapting to new cultures and learning a new language while working in Japan. Furthermore, the applicant has emphasized the desire to work with a team and the willingness to learn new skills, aligning with the company's soft skills requirements. The applicant's proactive approach to addressing weaknesses and ability to bridge technical and creative aspects in projects reflect an adaptable and team-oriented nature. Overall, the applicant's responses indicate a strong willingness to work in Japan and possess the necessary soft skills for the job.</t>
+          <t>The candidate has demonstrated strong adaptability, communication skills, and a willingness to embrace new challenges, as evidenced by the responses. The candidate's eagerness to work in Japan, learn a new language, and contribute to cutting-edge AI/ML technologies aligns with the company's values and culture. Furthermore, the applicant's proactive approach to addressing weaknesses and commitment to collaborative problem-solving reflect strong teamwork and problem-solving abilities. Overall, the candidate's responses indicate a high level of enthusiasm, adaptability, and alignment with the company's soft skill requirements, warranting a score of 4.</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The applicant possesses strong skills in Python, PyTorch, Tensorflow, and ReactJS, demonstrating proficiency in web and mobile application development. While the applicant's projects showcase extensive experience in computer vision, image processing, and backend development, there is a lack of direct experience with MongoDB, ExpressJS, and NodeJS, which are essential for the role. However, the applicant's versatility and experience in developing web applications using ReactJS could contribute to the role's responsibilities. Despite the gaps in experience with specific technologies, the applicant's strong foundation in relevant areas positions them as a promising candidate for the SDE Intern position.</t>
+          <t>The applicant has strong skills in Python, PyTorch, Django Rest Framework, and ReactJS, which are utilized in the projects 'LLMGuard', 'Multi Model Data Analysis for Annotation of Human Activities', and 'Website for the Literature Society of the college'. These projects demonstrate the applicant's proficiency in web development, machine learning, and backend development. However, the applicant lacks direct experience with MongoDB, ExpressJS, and NodeJS, which are the primary technologies mentioned in the job description. While the applicant's skills are impressive, there is a gap in the required MERN stack technologies, which may affect the ability to seamlessly transition to the role without additional training or orientation.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The applicant has exhibited a keen interest in being part of Japan's work culture, showcasing adaptability and a willingness to learn a new language while working in Japan. The applicant's responses convey a strong sense of commitment to pursuing a stable career in the field of AI/ML and backend development, aligning with the company's requirements. Furthermore, the applicant's acknowledgement of strengths in teamwork and openness about areas for improvement demonstrates a growth mindset and a potential for future development. Overall, the applicant's responses indicate a positive attitude and willingness to embrace the opportunities presented in Japan.</t>
+          <t>The applicant has exhibited a strong willingness to work in Japan by expressing interest in the AI field and the work culture of Japan. The applicant has shown adaptability by expressing a willingness to work in different countries, including Japan, and has highlighted the desire to learn a new language while working in Japan. Furthermore, the applicant has articulated the expectation of contributing to cutting-edge AI/ML technologies and learning new skills during the internship. The responses indicate good communication skills and a positive attitude towards teamwork and adaptability, aligning with the company's soft skill requirements.</t>
         </is>
       </c>
     </row>
@@ -532,15 +532,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The applicant has worked on various web development projects such as a Video Conferencing Project, TEDxIITGuwahati Website, and Alcheringa Pass Portal, showcasing strong skills in JavaScript, HTML, and CSS. However, the job requires expertise in MongoDB, ReactJS, and NodeJS, which are not fully exhibited in the applicant's projects. While the applicant's experience in web development is commendable, there is a lack of direct experience with the specific technologies mentioned in the job description. This indicates potential gaps in the applicant's skillset with regards to the technologies required for the job.</t>
+          <t>The applicant has showcased proficiency in JavaScript, HTML, CSS, and API integration through their projects. These skills align well with the company's requirements for web development. However, the applicant's lack of experience in MongoDB, ExpressJS, and NodeJS could be a limiting factor as the job specifically requires knowledge of these technologies. While the applicant's projects demonstrate strong front-end development skills, the absence of back-end technology experience is a gap that needs to be addressed for this role. It's crucial for an SDE Intern in MERN stack development to possess comprehensive knowledge across the entire stack, which is currently lacking in the applicant's skill set.</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The applicant has demonstrated an eagerness to work in Japan, expressing a genuine interest in the country's work culture and a willingness to adapt to a new environment. The applicant's openness to working in diverse locations demonstrates adaptability. Furthermore, the applicant's acknowledgment of strengths in teamwork aligns with the company's soft skill requirements. However, the applicant's admission of struggles with acquiring new skills and preference for working in a team may indicate a need for further development in individual problem-solving and time management skills, resulting in a score of 3 out of 5.</t>
+          <t>The applicant displayed a strong willingness to work in Japan and adapt to a new culture. Their enthusiasm for Japan's AI advancements, interest in learning the Japanese language, and admiration for Japanese work culture demonstrate a high level of adaptability and openness. Additionally, the applicant's emphasis on wanting a stable job, expectations of a decent package, and focus on contributing to cutting-edge AI/ML technologies align with the company's objectives. The candidate's proactive approach to overcoming weaknesses and their experience in problem-solving within a team further indicate strong adaptability, teamwork, and problem-solving skills. Based on the provided answers, the applicant exhibits a positive attitude and a genuine interest in working in Japan.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
puts back wrapper functions
</commit_message>
<xml_diff>
--- a/main/results/jdk_1.xlsx
+++ b/main/results/jdk_1.xlsx
@@ -465,11 +465,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>76.95</v>
+        <v>74.02</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The applicant possesses several key skills required by the company such as ReactJS, JavaScript, and some level of web development experience. While the applicant's projects are not directly in line with the company's requirements, the projects demonstrate a strong grasp of relevant technologies including ReactJS, Django, Python, JavaScript, and Computer Vision. However, the applicant lacks direct experience with MongoDB and NodeJS which are important for this role. Overall, the applicant has a good foundation in relevant technologies and has demonstrated the ability to learn new skills, presenting a strong case for potential success in the role.</t>
+          <t>The applicant possesses strong skills in TensorFlow, JavaScript, Scikit-learn, and Python which are crucial for the job role. Additionally, the applicant has experience in Django, ReactJS, and image processing, showcasing versatility and adaptability. However, the applicant lacks experience in PyTorch, and this could be a skill gap for the role. Nevertheless, the applicant's proficiency in Computer Vision and data analysis complements the job requirements, making the applicant a suitable candidate overall.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The applicant demonstrates strong communication skills and a willingness to learn from Japanese work culture, indicating adaptability and a positive attitude towards working in Japan. Moreover, the applicant's emphasis on seeking feedback, continuous self-improvement, and desire to experience Japanese cultural values align well with the company's soft skills requirements. The applicant's clear expression of interest in working in Japan further strengthens the likelihood of successful integration into the work culture.</t>
+          <t>The applicant has exhibited a proactive and adaptable personality during the interview process, showcasing a willingness to embrace new opportunities. Their responses also indicate an open-minded approach and a high level of flexibility, which align with the soft skills required by the company. Overall, the applicant demonstrates a strong willingness to work in Japan, making them a good fit for the company's international expansion plans.</t>
         </is>
       </c>
     </row>
@@ -486,11 +486,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>89.06999999999999</v>
+        <v>89.42</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The candidate has a strong technical background with experience in web and mobile application development utilizing technologies such as Flutter, Dart, Firebase, ReactJS, NodeJS, HTML, CSS, and WebRTC. Although the applicant's project experience primarily involves technologies such as Flutter, Dart, and Firebase, the candidate has demonstrated adaptability by working on a variety of projects involving different technology stacks. However, the required skills for the role include MongoDB, ExpressJS, and JavaScript, which are not directly reflected in the candidate's projects. While the candidate's projects showcase proficiency in relevant web and mobile technologies, there is a gap in direct experience with the specific technology stack mentioned in the job description. Despite this, the candidate's diverse skill set and demonstrated ability to learn new technologies provide a strong foundation for success in the role.</t>
+          <t>The applicant has experience with ReactJS, Flutter, and NodeJS which are essential for this job role. However, the applicant lacks experience with WebRTC, Socket.IO, and Docker, which are required by the company. Despite having some relevant skills, the lack of experience in these key areas makes the applicant less suited for this job position.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The candidate has demonstrated strong adaptability, communication skills, and a willingness to embrace new challenges, as evidenced by the responses. The candidate's eagerness to work in Japan, learn a new language, and contribute to cutting-edge AI/ML technologies aligns with the company's values and culture. Furthermore, the applicant's proactive approach to addressing weaknesses and commitment to collaborative problem-solving reflect strong teamwork and problem-solving abilities. Overall, the candidate's responses indicate a high level of enthusiasm, adaptability, and alignment with the company's soft skill requirements, warranting a score of 4.</t>
+          <t>The applicant has demonstrated strong communication skills and adaptability, making them suitable for the company's soft skill requirements. Additionally, the applicant has shown an eagerness to experience new cultures, which aligns with the company's focus on diversity and global perspectives.</t>
         </is>
       </c>
     </row>
@@ -507,11 +507,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>78.72</v>
+        <v>77.25</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>The applicant has strong skills in Python, PyTorch, Django Rest Framework, and ReactJS, which are utilized in the projects 'LLMGuard', 'Multi Model Data Analysis for Annotation of Human Activities', and 'Website for the Literature Society of the college'. These projects demonstrate the applicant's proficiency in web development, machine learning, and backend development. However, the applicant lacks direct experience with MongoDB, ExpressJS, and NodeJS, which are the primary technologies mentioned in the job description. While the applicant's skills are impressive, there is a gap in the required MERN stack technologies, which may affect the ability to seamlessly transition to the role without additional training or orientation.</t>
+          <t>The applicant possesses skills in PyTorch, TensorFlow, Django Rest Framework, Scikit-learn, and Keras, all of which are directly relevant to the job description provided by the company. The applicant also has experience in computer vision and image processing, which are additional valuable skills for the role. However, the applicant lacks experience in ReactJS and Python, which are among the required skills by the company. As a result, though the applicant has a strong background in the required technologies, the lack of experience in ReactJS and Python may impact the overall suitability for the role.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The applicant has exhibited a strong willingness to work in Japan by expressing interest in the AI field and the work culture of Japan. The applicant has shown adaptability by expressing a willingness to work in different countries, including Japan, and has highlighted the desire to learn a new language while working in Japan. Furthermore, the applicant has articulated the expectation of contributing to cutting-edge AI/ML technologies and learning new skills during the internship. The responses indicate good communication skills and a positive attitude towards teamwork and adaptability, aligning with the company's soft skill requirements.</t>
+          <t>The applicant has demonstrated good adaptability and openness to new experiences, which are essential qualities for working in a new environment such as Japan. Additionally, the applicant's responses indicated a high level of cultural awareness and respect, aligning well with the interpersonal skills sought by the company. Therefore, based on the applicant's personality traits and willingness to work in a new cultural setting, a score of 4 is justified.</t>
         </is>
       </c>
     </row>
@@ -528,11 +528,11 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>70.89</v>
+        <v>82.91</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>The applicant has showcased proficiency in JavaScript, HTML, CSS, and API integration through their projects. These skills align well with the company's requirements for web development. However, the applicant's lack of experience in MongoDB, ExpressJS, and NodeJS could be a limiting factor as the job specifically requires knowledge of these technologies. While the applicant's projects demonstrate strong front-end development skills, the absence of back-end technology experience is a gap that needs to be addressed for this role. It's crucial for an SDE Intern in MERN stack development to possess comprehensive knowledge across the entire stack, which is currently lacking in the applicant's skill set.</t>
+          <t>The applicant has relevant skills in API integration, JavaScript, HTML, and CSS, which align with the required skills set by the company. However, the applicant lacks experience in specific technologies mentioned in the job description, such as Python, Java, and AI/ML. While the projects demonstrate proficiency in web development, the absence of experience in the required technologies may limit the applicant's suitability for the role.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -540,7 +540,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The applicant displayed a strong willingness to work in Japan and adapt to a new culture. Their enthusiasm for Japan's AI advancements, interest in learning the Japanese language, and admiration for Japanese work culture demonstrate a high level of adaptability and openness. Additionally, the applicant's emphasis on wanting a stable job, expectations of a decent package, and focus on contributing to cutting-edge AI/ML technologies align with the company's objectives. The candidate's proactive approach to overcoming weaknesses and their experience in problem-solving within a team further indicate strong adaptability, teamwork, and problem-solving skills. Based on the provided answers, the applicant exhibits a positive attitude and a genuine interest in working in Japan.</t>
+          <t>The applicant exhibits a willingness to adapt and embrace new challenges, with a positive attitude towards relocation. Their responses reflect a strong sense of adaptability and open-mindedness, which are essential traits for thriving in a new environment. Moreover, the applicant demonstrates a keen interest in embracing the cultural aspects of Japan, indicating a genuine enthusiasm for the opportunity.</t>
         </is>
       </c>
     </row>

</xml_diff>